<commit_message>
Update on 30th April
</commit_message>
<xml_diff>
--- a/DB and Documents/OrageneSaliva.xlsx
+++ b/DB and Documents/OrageneSaliva.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
@@ -225,9 +225,6 @@
     <t>q51z3</t>
   </si>
   <si>
-    <t>Maternal Sample Collection Form – Section 2: Vital Signs Data Collection</t>
-  </si>
-  <si>
     <t>5.Mother Full Name</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t xml:space="preserve">2.P a rt i a l Aliquot </t>
+  </si>
+  <si>
+    <t>Maternal Sample Collection Form – Section 4: Oragene Saliva Sample Collection</t>
   </si>
 </sst>
 </file>
@@ -1777,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V19"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AR3" sqref="AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1895,7 +1895,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'dataid','frmHHID', 'tblMainQues','AvBwW bs:','Id no. :','','msg1','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="15" customFormat="1" ht="60">
+    <row r="3" spans="1:22" s="15" customFormat="1" ht="75">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1908,7 +1908,7 @@
       <c r="D3" s="21"/>
       <c r="E3" s="12"/>
       <c r="F3" s="17" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>59</v>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="V3" s="15" t="str">
         <f t="shared" ref="V3:V19" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'msg1','frmmessage', '','','Maternal Sample Collection Form – Section 2: Vital Signs Data Collection','','q2_3','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'msg1','frmmessage', '','','Maternal Sample Collection Form – Section 4: Oragene Saliva Sample Collection','','q2_3','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="31.5">
@@ -2015,7 +2015,7 @@
         <v>35</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>46</v>
@@ -2049,7 +2049,7 @@
         <v>35</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>47</v>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>39</v>
@@ -2108,7 +2108,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>30</v>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>39</v>
@@ -2151,7 +2151,7 @@
         <v>35</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>49</v>
@@ -2185,7 +2185,7 @@
         <v>35</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>50</v>
@@ -2219,7 +2219,7 @@
         <v>35</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>51</v>
@@ -2253,7 +2253,7 @@
         <v>35</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" s="21" t="s">
         <v>52</v>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="21" t="s">
         <v>53</v>
@@ -2321,7 +2321,7 @@
         <v>35</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" s="21" t="s">
         <v>54</v>
@@ -2346,7 +2346,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>30</v>
@@ -2355,7 +2355,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H16" s="21" t="s">
         <v>54</v>
@@ -2389,7 +2389,7 @@
         <v>35</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>55</v>
@@ -2423,7 +2423,7 @@
         <v>35</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>56</v>
@@ -2457,7 +2457,7 @@
         <v>35</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>39</v>
@@ -2988,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G20"/>
     </sheetView>
   </sheetViews>
@@ -3075,7 +3075,7 @@
         <v>47</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="15">
         <v>1</v>
@@ -3093,7 +3093,7 @@
         <v>47</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="33">
         <v>2</v>
@@ -3111,7 +3111,7 @@
         <v>47</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="33">
         <v>3</v>
@@ -3129,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="33">
         <v>4</v>
@@ -3147,7 +3147,7 @@
         <v>47</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="33">
         <v>5</v>
@@ -3165,13 +3165,13 @@
         <v>47</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="33">
         <v>6</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="15" t="str">
         <f t="shared" si="0"/>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="C12"/>
       <c r="D12" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="C13"/>
       <c r="D13" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="C14"/>
       <c r="D14" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="C15"/>
       <c r="D15" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="C16"/>
       <c r="D16" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -3323,13 +3323,13 @@
       </c>
       <c r="C17"/>
       <c r="D17" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G17" s="15" t="str">
         <f t="shared" si="0"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="C18"/>
       <c r="D18" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="C19"/>
       <c r="D19" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -3383,7 +3383,7 @@
       </c>
       <c r="C20"/>
       <c r="D20" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20">
         <v>3</v>

</xml_diff>